<commit_message>
add streamlit auth + config and update requirements
</commit_message>
<xml_diff>
--- a/data/2025/Q4预告/B/B.xlsx
+++ b/data/2025/Q4预告/B/B.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,3096 +492,3960 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>000100.SZ</t>
+          <t>000032.SZ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TCL科技</t>
+          <t>深桑达A</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D2" t="n">
-        <v>28.9</v>
+        <v>-3.8</v>
       </c>
       <c r="E2" t="n">
-        <v>990.1</v>
+        <v>264.7</v>
       </c>
       <c r="F2" t="n">
-        <v>4.6</v>
+        <v>0.7</v>
       </c>
       <c r="G2" t="n">
-        <v>-2.072</v>
+        <v>-0.8070000000000001</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.47</v>
+        <v>-1.199</v>
       </c>
       <c r="I2" t="n">
-        <v>34.3</v>
+        <v>-68.8</v>
       </c>
       <c r="J2" t="n">
-        <v>43.9</v>
+        <v>-193.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>000738.SZ</t>
+          <t>000430.SZ</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>航发控制</t>
+          <t>*ST张股</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D3" t="n">
-        <v>3.1</v>
+        <v>-5.3</v>
       </c>
       <c r="E3" t="n">
-        <v>298.8</v>
+        <v>60.5</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.8</v>
+        <v>-5</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.734</v>
+        <v>-0.033</v>
       </c>
       <c r="H3" t="n">
-        <v>-1.943</v>
+        <v>-1880.538</v>
       </c>
       <c r="I3" t="n">
-        <v>96.40000000000001</v>
+        <v>-11.4</v>
       </c>
       <c r="J3" t="n">
-        <v>-183.9</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>001283.SZ</t>
+          <t>000859.SZ</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>豪鹏科技</t>
+          <t>国风新材</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D4" t="n">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="E4" t="n">
-        <v>69.5</v>
+        <v>110.9</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="G4" t="n">
-        <v>0.367</v>
+        <v>-11.325</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.78</v>
+        <v>-0.199</v>
       </c>
       <c r="I4" t="n">
-        <v>38.6</v>
+        <v>-116.8</v>
       </c>
       <c r="J4" t="n">
-        <v>51</v>
+        <v>-119.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>002107.SZ</t>
+          <t>001212.SZ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>沃华医药</t>
+          <t>中旗新材</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8</v>
+        <v>-0.4</v>
       </c>
       <c r="E5" t="n">
-        <v>41.4</v>
+        <v>97.3</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1</v>
+        <v>-0.4</v>
       </c>
       <c r="G5" t="n">
-        <v>0.051</v>
+        <v>3.447</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.259</v>
+        <v>-325.786</v>
       </c>
       <c r="I5" t="n">
-        <v>55.2</v>
+        <v>-246.2</v>
       </c>
       <c r="J5" t="n">
-        <v>69.3</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>002240.SZ</t>
+          <t>002299.SZ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>盛新锂能</t>
+          <t>圣农发展</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D6" t="n">
-        <v>-7.5</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>343.3</v>
+        <v>200.4</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.276</v>
+        <v>-0.387</v>
       </c>
       <c r="H6" t="n">
-        <v>0.464</v>
+        <v>-0.229</v>
       </c>
       <c r="I6" t="n">
-        <v>-45.8</v>
+        <v>24.1</v>
       </c>
       <c r="J6" t="n">
-        <v>108.9</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>002879.SZ</t>
+          <t>002405.SZ</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>长缆科技</t>
+          <t>四维图新</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D7" t="n">
-        <v>1.2</v>
+        <v>-15.1</v>
       </c>
       <c r="E7" t="n">
-        <v>36.4</v>
+        <v>250.8</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9</v>
+        <v>-7.9</v>
       </c>
       <c r="G7" t="n">
-        <v>4.787</v>
+        <v>0.276</v>
       </c>
       <c r="H7" t="n">
-        <v>47.748</v>
+        <v>0.958</v>
       </c>
       <c r="I7" t="n">
-        <v>30.2</v>
+        <v>-16.6</v>
       </c>
       <c r="J7" t="n">
-        <v>13.4</v>
+        <v>-9.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>600135.SH</t>
+          <t>002534.SZ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>乐凯胶片</t>
+          <t>西子洁能</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.3</v>
+        <v>2.2</v>
       </c>
       <c r="E8" t="n">
-        <v>65.8</v>
+        <v>147.1</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3</v>
+        <v>0.7</v>
       </c>
       <c r="G8" t="n">
-        <v>0.266</v>
+        <v>-3.745</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.235</v>
+        <v>2.266</v>
       </c>
       <c r="I8" t="n">
-        <v>-49.7</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="J8" t="n">
-        <v>-49.2</v>
+        <v>63.7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>600231.SH</t>
+          <t>002969.SZ</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>凌钢股份</t>
+          <t>嘉美包装</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D9" t="n">
-        <v>-16.8</v>
+        <v>0.8</v>
       </c>
       <c r="E9" t="n">
-        <v>61.8</v>
+        <v>194.1</v>
       </c>
       <c r="F9" t="n">
-        <v>-8.4</v>
+        <v>0.4</v>
       </c>
       <c r="G9" t="n">
-        <v>1.535</v>
+        <v>-0.622</v>
       </c>
       <c r="H9" t="n">
-        <v>2.077</v>
+        <v>1.191</v>
       </c>
       <c r="I9" t="n">
-        <v>-3.7</v>
+        <v>252.6</v>
       </c>
       <c r="J9" t="n">
-        <v>-2.2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>600588.SH</t>
+          <t>300723.SZ</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>用友网络</t>
+          <t>一品红</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D10" t="n">
-        <v>-15.4</v>
+        <v>-4.7</v>
       </c>
       <c r="E10" t="n">
-        <v>590.5</v>
+        <v>188.6</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.6</v>
+        <v>-3</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.892</v>
+        <v>0.01</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.872</v>
+        <v>3.168</v>
       </c>
       <c r="I10" t="n">
-        <v>-38.3</v>
+        <v>-39.7</v>
       </c>
       <c r="J10" t="n">
-        <v>-91</v>
+        <v>-19.7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>601015.SH</t>
+          <t>600403.SH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>陕西黑猫</t>
+          <t>大有能源</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D11" t="n">
-        <v>-12.2</v>
+        <v>-18.4</v>
       </c>
       <c r="E11" t="n">
-        <v>80.90000000000001</v>
+        <v>183.4</v>
       </c>
       <c r="F11" t="n">
-        <v>-4.1</v>
+        <v>-6.8</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.143</v>
+        <v>0.947</v>
       </c>
       <c r="H11" t="n">
-        <v>0.454</v>
+        <v>1.411</v>
       </c>
       <c r="I11" t="n">
-        <v>-6.6</v>
+        <v>-10</v>
       </c>
       <c r="J11" t="n">
-        <v>-5.3</v>
+        <v>-7.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>603773.SH</t>
+          <t>601588.SH</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>沃格光电</t>
+          <t>北辰实业</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.6</v>
+        <v>-33.7</v>
       </c>
       <c r="E12" t="n">
-        <v>77.3</v>
+        <v>59.6</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.8</v>
+        <v>-11.6</v>
       </c>
       <c r="G12" t="n">
-        <v>0.175</v>
+        <v>-0.41</v>
       </c>
       <c r="H12" t="n">
-        <v>4.559</v>
+        <v>0.926</v>
       </c>
       <c r="I12" t="n">
-        <v>-48.3</v>
+        <v>-1.8</v>
       </c>
       <c r="J12" t="n">
-        <v>-29.7</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>605499.SH</t>
+          <t>601798.SH</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>东鹏饮料</t>
+          <t>蓝科高新</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D13" t="n">
-        <v>41.2</v>
+        <v>0.3</v>
       </c>
       <c r="E13" t="n">
-        <v>1417.6</v>
+        <v>32.9</v>
       </c>
       <c r="F13" t="n">
-        <v>5.8</v>
+        <v>0.1</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.032</v>
+        <v>-1.072</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.543</v>
+        <v>-0.46</v>
       </c>
       <c r="I13" t="n">
-        <v>34.4</v>
+        <v>107.3</v>
       </c>
       <c r="J13" t="n">
-        <v>47.1</v>
+        <v>125.3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>688525.SH</t>
+          <t>601992.SH</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>佰维存储</t>
+          <t>金隅集团</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="D14" t="n">
-        <v>7.6</v>
+        <v>-37.5</v>
       </c>
       <c r="E14" t="n">
-        <v>632.4</v>
+        <v>249.9</v>
       </c>
       <c r="F14" t="n">
-        <v>7.8</v>
+        <v>-3.7</v>
       </c>
       <c r="G14" t="n">
-        <v>-5.94</v>
+        <v>-0.413</v>
       </c>
       <c r="H14" t="n">
-        <v>2.649</v>
+        <v>-0.6830000000000001</v>
       </c>
       <c r="I14" t="n">
-        <v>83.2</v>
+        <v>-6.7</v>
       </c>
       <c r="J14" t="n">
-        <v>24.8</v>
+        <v>-10.9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>000408.SZ</t>
+          <t>603061.SH</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>藏格矿业</t>
+          <t>金海通</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D15" t="n">
-        <v>38.7</v>
+        <v>1.6</v>
       </c>
       <c r="E15" t="n">
-        <v>1341.1</v>
+        <v>120</v>
       </c>
       <c r="F15" t="n">
-        <v>11.1</v>
+        <v>0.3</v>
       </c>
       <c r="G15" t="n">
-        <v>0.59</v>
+        <v>0.115</v>
       </c>
       <c r="H15" t="n">
-        <v>0.175</v>
+        <v>-0.297</v>
       </c>
       <c r="I15" t="n">
-        <v>34.7</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="J15" t="n">
-        <v>31.3</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>002284.SZ</t>
+          <t>603186.SH</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>亚太股份</t>
+          <t>华正新材</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D16" t="n">
-        <v>4.2</v>
+        <v>0.6</v>
       </c>
       <c r="E16" t="n">
-        <v>114.8</v>
+        <v>77.3</v>
       </c>
       <c r="F16" t="n">
-        <v>1.3</v>
+        <v>0.1</v>
       </c>
       <c r="G16" t="n">
-        <v>1.426</v>
+        <v>-1.096</v>
       </c>
       <c r="H16" t="n">
-        <v>0.227</v>
+        <v>-0.32</v>
       </c>
       <c r="I16" t="n">
-        <v>27.2</v>
+        <v>128.8</v>
       </c>
       <c r="J16" t="n">
-        <v>22.8</v>
+        <v>166.3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>002345.SZ</t>
+          <t>603818.SH</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>潮宏基</t>
+          <t>曲美家居</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D17" t="n">
-        <v>4.2</v>
+        <v>-1.4</v>
       </c>
       <c r="E17" t="n">
-        <v>110.9</v>
+        <v>25.2</v>
       </c>
       <c r="F17" t="n">
-        <v>1.1</v>
+        <v>-0.3</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.873</v>
+        <v>-0.174</v>
       </c>
       <c r="H17" t="n">
-        <v>-7.933</v>
+        <v>0.001</v>
       </c>
       <c r="I17" t="n">
-        <v>26.3</v>
+        <v>-17.4</v>
       </c>
       <c r="J17" t="n">
-        <v>36.2</v>
+        <v>-18.6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>002459.SZ</t>
+          <t>603956.SH</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>晶澳科技</t>
+          <t>威派格</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D18" t="n">
-        <v>-51</v>
+        <v>-1.5</v>
       </c>
       <c r="E18" t="n">
-        <v>403.1</v>
+        <v>40.2</v>
       </c>
       <c r="F18" t="n">
-        <v>-16.5</v>
+        <v>-0.7</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.552</v>
+        <v>-0.041</v>
       </c>
       <c r="H18" t="n">
-        <v>0.413</v>
+        <v>-10.356</v>
       </c>
       <c r="I18" t="n">
-        <v>-7.9</v>
+        <v>-26.7</v>
       </c>
       <c r="J18" t="n">
-        <v>-6.6</v>
+        <v>-20.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>002942.SZ</t>
+          <t>603992.SH</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>新农股份</t>
+          <t>松霖科技</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7</v>
+        <v>1.6</v>
       </c>
       <c r="E19" t="n">
-        <v>31.7</v>
+        <v>192.8</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G19" t="n">
-        <v>0.006</v>
+        <v>-0.761</v>
       </c>
       <c r="H19" t="n">
-        <v>-3.264</v>
+        <v>-0.481</v>
       </c>
       <c r="I19" t="n">
-        <v>46.6</v>
+        <v>124.4</v>
       </c>
       <c r="J19" t="n">
-        <v>-58.2</v>
+        <v>136.3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>300782.SZ</t>
+          <t>605006.SH</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>卓胜微</t>
+          <t>山东玻纤</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D20" t="n">
-        <v>-3.4</v>
+        <v>-0.3</v>
       </c>
       <c r="E20" t="n">
-        <v>453.3</v>
+        <v>44.1</v>
       </c>
       <c r="F20" t="n">
-        <v>-1.3</v>
+        <v>-0.2</v>
       </c>
       <c r="G20" t="n">
-        <v>1.572</v>
+        <v>-0.49</v>
       </c>
       <c r="H20" t="n">
-        <v>1.426</v>
+        <v>0.043</v>
       </c>
       <c r="I20" t="n">
-        <v>-134.9</v>
+        <v>-133.1</v>
       </c>
       <c r="J20" t="n">
-        <v>-101.6</v>
+        <v>-56.3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>600186.SH</t>
+          <t>605020.SH</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>莲花控股</t>
+          <t>永和股份</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D21" t="n">
-        <v>2.8</v>
+        <v>5.2</v>
       </c>
       <c r="E21" t="n">
-        <v>115.7</v>
+        <v>134.2</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.242</v>
+        <v>-0.359</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.681</v>
+        <v>-0.646</v>
       </c>
       <c r="I21" t="n">
-        <v>41.3</v>
+        <v>25.6</v>
       </c>
       <c r="J21" t="n">
-        <v>65.7</v>
+        <v>34.4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>600703.SH</t>
+          <t>605055.SH</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>三安光电</t>
+          <t>迎丰股份</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D22" t="n">
-        <v>-8.5</v>
+        <v>-0.5</v>
       </c>
       <c r="E22" t="n">
-        <v>788.3</v>
+        <v>42.8</v>
       </c>
       <c r="F22" t="n">
-        <v>-5.2</v>
+        <v>-0.2</v>
       </c>
       <c r="G22" t="n">
-        <v>2.26</v>
+        <v>-1.918</v>
       </c>
       <c r="H22" t="n">
-        <v>1.279</v>
+        <v>-0.2</v>
       </c>
       <c r="I22" t="n">
-        <v>-92.7</v>
+        <v>-80.7</v>
       </c>
       <c r="J22" t="n">
-        <v>-44</v>
+        <v>-66.90000000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>603259.SH</t>
+          <t>688126.SH</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>药明康德</t>
+          <t>沪硅产业</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D23" t="n">
-        <v>132.4</v>
+        <v>-18</v>
       </c>
       <c r="E23" t="n">
-        <v>2944.4</v>
+        <v>752.9</v>
       </c>
       <c r="F23" t="n">
-        <v>37.2</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>0.125</v>
+        <v>0.632</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.056</v>
+        <v>1.852</v>
       </c>
       <c r="I23" t="n">
-        <v>22.2</v>
+        <v>-41.8</v>
       </c>
       <c r="J23" t="n">
-        <v>19.5</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>603663.SH</t>
+          <t>688528.SH</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>三祥新材</t>
+          <t>秦川物联</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9</v>
+        <v>-1.2</v>
       </c>
       <c r="E24" t="n">
-        <v>157.5</v>
+        <v>19</v>
       </c>
       <c r="F24" t="n">
-        <v>0.2</v>
+        <v>-0.5</v>
       </c>
       <c r="G24" t="n">
-        <v>2.882</v>
+        <v>0.898</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.515</v>
+        <v>4.27</v>
       </c>
       <c r="I24" t="n">
-        <v>169.3</v>
+        <v>-15.2</v>
       </c>
       <c r="J24" t="n">
-        <v>197.4</v>
+        <v>-11.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>688005.SH</t>
+          <t>000100.SZ</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>容百科技</t>
+          <t>TCL科技</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="D25" t="n">
-        <v>-2.2</v>
+        <v>28.9</v>
       </c>
       <c r="E25" t="n">
-        <v>262.6</v>
+        <v>990.1</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.995</v>
+        <v>-2.072</v>
       </c>
       <c r="H25" t="n">
-        <v>-1.006</v>
+        <v>-0.47</v>
       </c>
       <c r="I25" t="n">
-        <v>-119.4</v>
+        <v>34.3</v>
       </c>
       <c r="J25" t="n">
-        <v>-188.8</v>
+        <v>43.9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>688192.SH</t>
+          <t>000738.SZ</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>迪哲医药-U</t>
+          <t>航发控制</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="D26" t="n">
-        <v>-8.5</v>
+        <v>3.1</v>
       </c>
       <c r="E26" t="n">
-        <v>308.7</v>
+        <v>298.8</v>
       </c>
       <c r="F26" t="n">
-        <v>-2.2</v>
+        <v>-0.8</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.267</v>
+        <v>-1.734</v>
       </c>
       <c r="H26" t="n">
-        <v>0.037</v>
+        <v>-1.943</v>
       </c>
       <c r="I26" t="n">
-        <v>-36.3</v>
+        <v>96.40000000000001</v>
       </c>
       <c r="J26" t="n">
-        <v>-35.5</v>
+        <v>-183.9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>300122.SZ</t>
+          <t>001283.SZ</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>智飞生物</t>
+          <t>豪鹏科技</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>46034</v>
+        <v>46036</v>
       </c>
       <c r="D27" t="n">
-        <v>-135.4</v>
+        <v>1.8</v>
       </c>
       <c r="E27" t="n">
-        <v>474</v>
+        <v>69.5</v>
       </c>
       <c r="F27" t="n">
-        <v>-123.1</v>
+        <v>0.2</v>
       </c>
       <c r="G27" t="n">
-        <v>80.286</v>
+        <v>0.367</v>
       </c>
       <c r="H27" t="n">
-        <v>19.291</v>
+        <v>-0.78</v>
       </c>
       <c r="I27" t="n">
-        <v>-3.5</v>
+        <v>38.6</v>
       </c>
       <c r="J27" t="n">
-        <v>-1.3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>300926.SZ</t>
+          <t>002107.SZ</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>博俊科技</t>
+          <t>沃华医药</t>
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>46034</v>
+        <v>46036</v>
       </c>
       <c r="D28" t="n">
-        <v>8.300000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="E28" t="n">
-        <v>143.4</v>
+        <v>41.4</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.179</v>
+        <v>0.051</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.266</v>
+        <v>-0.259</v>
       </c>
       <c r="I28" t="n">
-        <v>17.4</v>
+        <v>55.2</v>
       </c>
       <c r="J28" t="n">
-        <v>16.3</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>600990.SH</t>
+          <t>002240.SZ</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>四创电子</t>
+          <t>盛新锂能</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>46034</v>
+        <v>46036</v>
       </c>
       <c r="D29" t="n">
-        <v>-3.5</v>
+        <v>-7.5</v>
       </c>
       <c r="E29" t="n">
-        <v>94.8</v>
+        <v>343.3</v>
       </c>
       <c r="F29" t="n">
-        <v>-2.5</v>
+        <v>0.9</v>
       </c>
       <c r="G29" t="n">
-        <v>0.08799999999999999</v>
+        <v>-1.276</v>
       </c>
       <c r="H29" t="n">
-        <v>4.223</v>
+        <v>0.464</v>
       </c>
       <c r="I29" t="n">
-        <v>-27.1</v>
+        <v>-45.8</v>
       </c>
       <c r="J29" t="n">
-        <v>-11.7</v>
+        <v>108.9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>605555.SH</t>
+          <t>002879.SZ</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>德昌股份</t>
+          <t>长缆科技</t>
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>46034</v>
+        <v>46036</v>
       </c>
       <c r="D30" t="n">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="E30" t="n">
-        <v>90.7</v>
+        <v>36.4</v>
       </c>
       <c r="F30" t="n">
-        <v>-0</v>
+        <v>0.9</v>
       </c>
       <c r="G30" t="n">
-        <v>-1.038</v>
+        <v>4.787</v>
       </c>
       <c r="H30" t="n">
-        <v>-1.08</v>
+        <v>47.748</v>
       </c>
       <c r="I30" t="n">
-        <v>62.4</v>
+        <v>30.2</v>
       </c>
       <c r="J30" t="n">
-        <v>235.6</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>600501.SH</t>
+          <t>600135.SH</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>航天晨光</t>
+          <t>乐凯胶片</t>
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D31" t="n">
-        <v>-2.1</v>
+        <v>-1.3</v>
       </c>
       <c r="E31" t="n">
-        <v>156.5</v>
+        <v>65.8</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.9</v>
+        <v>-0.3</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.63</v>
+        <v>0.266</v>
       </c>
       <c r="H31" t="n">
-        <v>1.561</v>
+        <v>-0.235</v>
       </c>
       <c r="I31" t="n">
-        <v>-74.5</v>
+        <v>-49.7</v>
       </c>
       <c r="J31" t="n">
-        <v>-53.3</v>
+        <v>-49.2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>600606.SH</t>
+          <t>600231.SH</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>绿地控股</t>
+          <t>凌钢股份</t>
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D32" t="n">
-        <v>-189.5</v>
+        <v>-16.8</v>
       </c>
       <c r="E32" t="n">
-        <v>240.3</v>
+        <v>61.8</v>
       </c>
       <c r="F32" t="n">
-        <v>-129.1</v>
+        <v>-8.4</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.08400000000000001</v>
+        <v>1.535</v>
       </c>
       <c r="H32" t="n">
-        <v>3.389</v>
+        <v>2.077</v>
       </c>
       <c r="I32" t="n">
-        <v>-1.3</v>
+        <v>-3.7</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.6</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>600685.SH</t>
+          <t>600588.SH</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>中船防务</t>
+          <t>用友网络</t>
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D33" t="n">
-        <v>8.5</v>
+        <v>-15.4</v>
       </c>
       <c r="E33" t="n">
-        <v>442.3</v>
+        <v>590.5</v>
       </c>
       <c r="F33" t="n">
-        <v>2.4</v>
+        <v>-0.6</v>
       </c>
       <c r="G33" t="n">
-        <v>0.393</v>
+        <v>-0.892</v>
       </c>
       <c r="H33" t="n">
-        <v>1.146</v>
+        <v>-0.872</v>
       </c>
       <c r="I33" t="n">
-        <v>52</v>
+        <v>-38.3</v>
       </c>
       <c r="J33" t="n">
-        <v>52.1</v>
+        <v>-91</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>688208.SH</t>
+          <t>601015.SH</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>道通科技</t>
+          <t>陕西黑猫</t>
         </is>
       </c>
       <c r="C34" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D34" t="n">
-        <v>8.699999999999999</v>
+        <v>-12.2</v>
       </c>
       <c r="E34" t="n">
-        <v>250.6</v>
+        <v>80.90000000000001</v>
       </c>
       <c r="F34" t="n">
-        <v>1.5</v>
+        <v>-4.1</v>
       </c>
       <c r="G34" t="n">
-        <v>0.5659999999999999</v>
+        <v>-0.143</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.374</v>
+        <v>0.454</v>
       </c>
       <c r="I34" t="n">
-        <v>28.8</v>
+        <v>-6.6</v>
       </c>
       <c r="J34" t="n">
-        <v>35.8</v>
+        <v>-5.3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>688508.SH</t>
+          <t>603773.SH</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>芯朋微</t>
+          <t>沃格光电</t>
         </is>
       </c>
       <c r="C35" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6</v>
+        <v>-1.6</v>
       </c>
       <c r="E35" t="n">
-        <v>85</v>
+        <v>77.3</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.2</v>
+        <v>-0.8</v>
       </c>
       <c r="G35" t="n">
-        <v>-3.655</v>
+        <v>0.175</v>
       </c>
       <c r="H35" t="n">
-        <v>-5.723</v>
+        <v>4.559</v>
       </c>
       <c r="I35" t="n">
-        <v>154.5</v>
+        <v>-48.3</v>
       </c>
       <c r="J35" t="n">
-        <v>-178.7</v>
+        <v>-29.7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>688660.SH</t>
+          <t>605499.SH</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>电气风电</t>
+          <t>东鹏饮料</t>
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D36" t="n">
-        <v>-11.3</v>
+        <v>41.2</v>
       </c>
       <c r="E36" t="n">
-        <v>239.9</v>
+        <v>1417.6</v>
       </c>
       <c r="F36" t="n">
-        <v>-3.8</v>
+        <v>5.8</v>
       </c>
       <c r="G36" t="n">
-        <v>0.152</v>
+        <v>-0.032</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.171</v>
+        <v>-0.543</v>
       </c>
       <c r="I36" t="n">
-        <v>-21.2</v>
+        <v>34.4</v>
       </c>
       <c r="J36" t="n">
-        <v>-15.1</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>688707.SH</t>
+          <t>688525.SH</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>振华新材</t>
+          <t>佰维存储</t>
         </is>
       </c>
       <c r="C37" s="2" t="n">
-        <v>46032</v>
+        <v>46036</v>
       </c>
       <c r="D37" t="n">
-        <v>-5.1</v>
+        <v>7.6</v>
       </c>
       <c r="E37" t="n">
-        <v>75.09999999999999</v>
+        <v>632.4</v>
       </c>
       <c r="F37" t="n">
-        <v>-1.7</v>
+        <v>7.8</v>
       </c>
       <c r="G37" t="n">
-        <v>-0.121</v>
+        <v>-5.94</v>
       </c>
       <c r="H37" t="n">
-        <v>0.485</v>
+        <v>2.649</v>
       </c>
       <c r="I37" t="n">
-        <v>-14.6</v>
+        <v>83.2</v>
       </c>
       <c r="J37" t="n">
-        <v>-11.8</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>688777.SH</t>
+          <t>000408.SZ</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>中控技术</t>
+          <t>藏格矿业</t>
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="D38" t="n">
-        <v>3.3</v>
+        <v>38.7</v>
       </c>
       <c r="E38" t="n">
-        <v>424.4</v>
+        <v>1341.1</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.1</v>
+        <v>11.1</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.028</v>
+        <v>0.59</v>
       </c>
       <c r="H38" t="n">
-        <v>-1.215</v>
+        <v>0.175</v>
       </c>
       <c r="I38" t="n">
-        <v>129.5</v>
+        <v>34.7</v>
       </c>
       <c r="J38" t="n">
-        <v>2416.8</v>
+        <v>31.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>002925.SZ</t>
+          <t>002284.SZ</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>盈趣科技</t>
+          <t>亚太股份</t>
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D39" t="n">
-        <v>2.2</v>
+        <v>4.2</v>
       </c>
       <c r="E39" t="n">
-        <v>156.1</v>
+        <v>114.8</v>
       </c>
       <c r="F39" t="n">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="G39" t="n">
-        <v>-0.445</v>
+        <v>1.426</v>
       </c>
       <c r="H39" t="n">
-        <v>0.363</v>
+        <v>0.227</v>
       </c>
       <c r="I39" t="n">
-        <v>71</v>
+        <v>27.2</v>
       </c>
       <c r="J39" t="n">
-        <v>80.2</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>300482.SZ</t>
+          <t>002345.SZ</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>万孚生物</t>
+          <t>潮宏基</t>
         </is>
       </c>
       <c r="C40" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.2</v>
+        <v>4.2</v>
       </c>
       <c r="E40" t="n">
-        <v>94.40000000000001</v>
+        <v>110.9</v>
       </c>
       <c r="F40" t="n">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.888</v>
+        <v>-1.873</v>
       </c>
       <c r="H40" t="n">
-        <v>0.377</v>
+        <v>-7.933</v>
       </c>
       <c r="I40" t="n">
-        <v>-629.4</v>
+        <v>26.3</v>
       </c>
       <c r="J40" t="n">
-        <v>-25.9</v>
+        <v>36.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>300627.SZ</t>
+          <t>002459.SZ</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>华测导航</t>
+          <t>晶澳科技</t>
         </is>
       </c>
       <c r="C41" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D41" t="n">
-        <v>6</v>
+        <v>-51</v>
       </c>
       <c r="E41" t="n">
-        <v>326.9</v>
+        <v>403.1</v>
       </c>
       <c r="F41" t="n">
-        <v>1.5</v>
+        <v>-16.5</v>
       </c>
       <c r="G41" t="n">
-        <v>-0.103</v>
+        <v>-0.552</v>
       </c>
       <c r="H41" t="n">
-        <v>-0.053</v>
+        <v>0.413</v>
       </c>
       <c r="I41" t="n">
-        <v>54.7</v>
+        <v>-7.9</v>
       </c>
       <c r="J41" t="n">
-        <v>55.4</v>
+        <v>-6.6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>300871.SZ</t>
+          <t>002942.SZ</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>回盛生物</t>
+          <t>新农股份</t>
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D42" t="n">
-        <v>2.1</v>
+        <v>0.7</v>
       </c>
       <c r="E42" t="n">
-        <v>45.4</v>
+        <v>31.7</v>
       </c>
       <c r="F42" t="n">
-        <v>0.5</v>
+        <v>-0.2</v>
       </c>
       <c r="G42" t="n">
-        <v>1.887</v>
+        <v>0.006</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.299</v>
+        <v>-3.264</v>
       </c>
       <c r="I42" t="n">
-        <v>21.4</v>
+        <v>46.6</v>
       </c>
       <c r="J42" t="n">
-        <v>22</v>
+        <v>-58.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>300887.SZ</t>
+          <t>300782.SZ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>谱尼测试</t>
+          <t>卓胜微</t>
         </is>
       </c>
       <c r="C43" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D43" t="n">
-        <v>-2.6</v>
+        <v>-3.4</v>
       </c>
       <c r="E43" t="n">
-        <v>87.2</v>
+        <v>453.3</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.6</v>
+        <v>-1.3</v>
       </c>
       <c r="G43" t="n">
-        <v>-0.5590000000000001</v>
+        <v>1.572</v>
       </c>
       <c r="H43" t="n">
-        <v>1.762</v>
+        <v>1.426</v>
       </c>
       <c r="I43" t="n">
-        <v>-33.4</v>
+        <v>-134.9</v>
       </c>
       <c r="J43" t="n">
-        <v>-44</v>
+        <v>-101.6</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>600340.SH</t>
+          <t>600186.SH</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>华夏幸福</t>
+          <t>莲花控股</t>
         </is>
       </c>
       <c r="C44" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D44" t="n">
-        <v>-250</v>
+        <v>2.8</v>
       </c>
       <c r="E44" t="n">
-        <v>89.59999999999999</v>
+        <v>115.7</v>
       </c>
       <c r="F44" t="n">
-        <v>-148.2</v>
+        <v>0.3</v>
       </c>
       <c r="G44" t="n">
-        <v>2.799</v>
+        <v>-0.242</v>
       </c>
       <c r="H44" t="n">
-        <v>4.994</v>
+        <v>-0.681</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.4</v>
+        <v>41.3</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.2</v>
+        <v>65.7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>601872.SH</t>
+          <t>600703.SH</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>招商轮船</t>
+          <t>三安光电</t>
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D45" t="n">
-        <v>50.1</v>
+        <v>-8.5</v>
       </c>
       <c r="E45" t="n">
-        <v>775.2</v>
+        <v>788.3</v>
       </c>
       <c r="F45" t="n">
-        <v>21</v>
+        <v>-5.2</v>
       </c>
       <c r="G45" t="n">
-        <v>0.218</v>
+        <v>2.26</v>
       </c>
       <c r="H45" t="n">
-        <v>1.115</v>
+        <v>1.279</v>
       </c>
       <c r="I45" t="n">
-        <v>15.5</v>
+        <v>-92.7</v>
       </c>
       <c r="J45" t="n">
-        <v>10.6</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>603895.SH</t>
+          <t>603259.SH</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>天永智能</t>
+          <t>药明康德</t>
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>132.4</v>
       </c>
       <c r="E46" t="n">
-        <v>33.5</v>
+        <v>2944.4</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.1</v>
+        <v>37.2</v>
       </c>
       <c r="G46" t="n">
-        <v>-0.961</v>
+        <v>0.125</v>
       </c>
       <c r="H46" t="n">
-        <v>-3.763</v>
+        <v>-0.056</v>
       </c>
       <c r="I46" t="n">
-        <v>836.3</v>
+        <v>22.2</v>
       </c>
       <c r="J46" t="n">
-        <v>-204.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>688362.SH</t>
+          <t>603663.SH</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>甬矽电子</t>
+          <t>三祥新材</t>
         </is>
       </c>
       <c r="C47" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E47" t="n">
-        <v>167.4</v>
+        <v>157.5</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.2</v>
+        <v>0.2</v>
       </c>
       <c r="G47" t="n">
-        <v>-20.432</v>
+        <v>2.882</v>
       </c>
       <c r="H47" t="n">
-        <v>-2.607</v>
+        <v>-0.515</v>
       </c>
       <c r="I47" t="n">
-        <v>-334.7</v>
+        <v>169.3</v>
       </c>
       <c r="J47" t="n">
-        <v>-388.9</v>
+        <v>197.4</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>300389.SZ</t>
+          <t>688005.SH</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>艾比森</t>
+          <t>容百科技</t>
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>46030</v>
+        <v>46035</v>
       </c>
       <c r="D48" t="n">
-        <v>2.2</v>
+        <v>-2.2</v>
       </c>
       <c r="E48" t="n">
-        <v>64.90000000000001</v>
+        <v>262.6</v>
       </c>
       <c r="F48" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>-21.933</v>
+        <v>-0.995</v>
       </c>
       <c r="H48" t="n">
-        <v>0.005</v>
+        <v>-1.006</v>
       </c>
       <c r="I48" t="n">
-        <v>29.6</v>
+        <v>-119.4</v>
       </c>
       <c r="J48" t="n">
-        <v>29</v>
+        <v>-188.8</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>300498.SZ</t>
+          <t>688192.SH</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>温氏股份</t>
+          <t>迪哲医药-U</t>
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>46030</v>
+        <v>46035</v>
       </c>
       <c r="D49" t="n">
-        <v>48</v>
+        <v>-8.5</v>
       </c>
       <c r="E49" t="n">
-        <v>1125.2</v>
+        <v>308.7</v>
       </c>
       <c r="F49" t="n">
-        <v>-0.9</v>
+        <v>-2.2</v>
       </c>
       <c r="G49" t="n">
-        <v>-1.029</v>
+        <v>-0.267</v>
       </c>
       <c r="H49" t="n">
-        <v>-1.054</v>
+        <v>0.037</v>
       </c>
       <c r="I49" t="n">
-        <v>23.4</v>
+        <v>-36.3</v>
       </c>
       <c r="J49" t="n">
-        <v>82.3</v>
+        <v>-35.5</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>300505.SZ</t>
+          <t>300122.SZ</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>川金诺</t>
+          <t>智飞生物</t>
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="D50" t="n">
-        <v>4.2</v>
+        <v>-135.4</v>
       </c>
       <c r="E50" t="n">
-        <v>65.09999999999999</v>
+        <v>474</v>
       </c>
       <c r="F50" t="n">
-        <v>1.2</v>
+        <v>-123.1</v>
       </c>
       <c r="G50" t="n">
-        <v>0.883</v>
+        <v>80.286</v>
       </c>
       <c r="H50" t="n">
-        <v>0.001</v>
+        <v>19.291</v>
       </c>
       <c r="I50" t="n">
-        <v>15.7</v>
+        <v>-3.5</v>
       </c>
       <c r="J50" t="n">
-        <v>13.1</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>300748.SZ</t>
+          <t>300926.SZ</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>金力永磁</t>
+          <t>博俊科技</t>
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="D51" t="n">
-        <v>5.8</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E51" t="n">
-        <v>502.2</v>
+        <v>143.4</v>
       </c>
       <c r="F51" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="G51" t="n">
-        <v>0.85</v>
+        <v>-0.179</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.236</v>
+        <v>-0.266</v>
       </c>
       <c r="I51" t="n">
-        <v>86.59999999999999</v>
+        <v>17.4</v>
       </c>
       <c r="J51" t="n">
-        <v>77.8</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>300905.SZ</t>
+          <t>600990.SH</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>宝丽迪</t>
+          <t>四创电子</t>
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="D52" t="n">
-        <v>1.4</v>
+        <v>-3.5</v>
       </c>
       <c r="E52" t="n">
-        <v>60.9</v>
+        <v>94.8</v>
       </c>
       <c r="F52" t="n">
-        <v>0.4</v>
+        <v>-2.5</v>
       </c>
       <c r="G52" t="n">
-        <v>0.186</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="H52" t="n">
-        <v>-0.089</v>
+        <v>4.223</v>
       </c>
       <c r="I52" t="n">
-        <v>43.2</v>
+        <v>-27.1</v>
       </c>
       <c r="J52" t="n">
-        <v>38.9</v>
+        <v>-11.7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>600189.SH</t>
+          <t>605555.SH</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>泉阳泉</t>
+          <t>德昌股份</t>
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>46030</v>
+        <v>46034</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.2</v>
+        <v>1.5</v>
       </c>
       <c r="E53" t="n">
-        <v>49.9</v>
+        <v>90.7</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.1</v>
+        <v>-0</v>
       </c>
       <c r="G53" t="n">
-        <v>-0.778</v>
+        <v>-1.038</v>
       </c>
       <c r="H53" t="n">
-        <v>0.046</v>
+        <v>-1.08</v>
       </c>
       <c r="I53" t="n">
-        <v>-316.8</v>
+        <v>62.4</v>
       </c>
       <c r="J53" t="n">
-        <v>-96</v>
+        <v>235.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>600435.SH</t>
+          <t>600501.SH</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>北方导航</t>
+          <t>航天晨光</t>
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D54" t="n">
-        <v>0.9</v>
+        <v>-2.1</v>
       </c>
       <c r="E54" t="n">
-        <v>299.7</v>
+        <v>156.5</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.3</v>
+        <v>-0.9</v>
       </c>
       <c r="G54" t="n">
-        <v>-1.216</v>
+        <v>-0.63</v>
       </c>
       <c r="H54" t="n">
-        <v>-6.115</v>
+        <v>1.561</v>
       </c>
       <c r="I54" t="n">
-        <v>336.8</v>
+        <v>-74.5</v>
       </c>
       <c r="J54" t="n">
-        <v>-382.5</v>
+        <v>-53.3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>600537.SH</t>
+          <t>600606.SH</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>亿晶光电</t>
+          <t>绿地控股</t>
         </is>
       </c>
       <c r="C55" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D55" t="n">
-        <v>-6</v>
+        <v>-189.5</v>
       </c>
       <c r="E55" t="n">
-        <v>51</v>
+        <v>240.3</v>
       </c>
       <c r="F55" t="n">
-        <v>-3.9</v>
+        <v>-129.1</v>
       </c>
       <c r="G55" t="n">
-        <v>-0.746</v>
+        <v>-0.08400000000000001</v>
       </c>
       <c r="H55" t="n">
-        <v>5.3</v>
+        <v>3.389</v>
       </c>
       <c r="I55" t="n">
-        <v>-8.5</v>
+        <v>-1.3</v>
       </c>
       <c r="J55" t="n">
-        <v>-4.2</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>603309.SH</t>
+          <t>600685.SH</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>维力医疗</t>
+          <t>中船防务</t>
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D56" t="n">
-        <v>0.6</v>
+        <v>8.5</v>
       </c>
       <c r="E56" t="n">
-        <v>41.4</v>
+        <v>442.3</v>
       </c>
       <c r="F56" t="n">
-        <v>-1.2</v>
+        <v>2.4</v>
       </c>
       <c r="G56" t="n">
-        <v>-3.387</v>
+        <v>0.393</v>
       </c>
       <c r="H56" t="n">
-        <v>-2.788</v>
+        <v>1.146</v>
       </c>
       <c r="I56" t="n">
-        <v>63.7</v>
+        <v>52</v>
       </c>
       <c r="J56" t="n">
-        <v>-14.2</v>
+        <v>52.1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>603588.SH</t>
+          <t>688208.SH</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>高能环境</t>
+          <t>道通科技</t>
         </is>
       </c>
       <c r="C57" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D57" t="n">
-        <v>7.5</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="E57" t="n">
-        <v>126.1</v>
+        <v>250.6</v>
       </c>
       <c r="F57" t="n">
         <v>1.5</v>
       </c>
       <c r="G57" t="n">
-        <v>-2.068</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="H57" t="n">
-        <v>0.037</v>
+        <v>-0.374</v>
       </c>
       <c r="I57" t="n">
-        <v>16.8</v>
+        <v>28.8</v>
       </c>
       <c r="J57" t="n">
-        <v>21.1</v>
+        <v>35.8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>603589.SH</t>
+          <t>688508.SH</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>口子窖</t>
+          <t>芯朋微</t>
         </is>
       </c>
       <c r="C58" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D58" t="n">
-        <v>6.5</v>
+        <v>0.6</v>
       </c>
       <c r="E58" t="n">
-        <v>181.3</v>
+        <v>85</v>
       </c>
       <c r="F58" t="n">
-        <v>-0.8</v>
+        <v>-0.2</v>
       </c>
       <c r="G58" t="n">
-        <v>-1.231</v>
+        <v>-3.655</v>
       </c>
       <c r="H58" t="n">
-        <v>-3.991</v>
+        <v>-5.723</v>
       </c>
       <c r="I58" t="n">
-        <v>28.1</v>
+        <v>154.5</v>
       </c>
       <c r="J58" t="n">
-        <v>-85.5</v>
+        <v>-178.7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>603590.SH</t>
+          <t>688660.SH</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>康辰药业</t>
+          <t>电气风电</t>
         </is>
       </c>
       <c r="C59" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D59" t="n">
-        <v>1.4</v>
+        <v>-11.3</v>
       </c>
       <c r="E59" t="n">
-        <v>66.59999999999999</v>
+        <v>239.9</v>
       </c>
       <c r="F59" t="n">
-        <v>0.1</v>
+        <v>-3.8</v>
       </c>
       <c r="G59" t="n">
-        <v>-1.093</v>
+        <v>0.152</v>
       </c>
       <c r="H59" t="n">
-        <v>-0.8100000000000001</v>
+        <v>-0.171</v>
       </c>
       <c r="I59" t="n">
-        <v>47.6</v>
+        <v>-21.2</v>
       </c>
       <c r="J59" t="n">
-        <v>115.4</v>
+        <v>-15.1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>688332.SH</t>
+          <t>688707.SH</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>中科蓝讯</t>
+          <t>振华新材</t>
         </is>
       </c>
       <c r="C60" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D60" t="n">
-        <v>2.2</v>
+        <v>-5.1</v>
       </c>
       <c r="E60" t="n">
-        <v>161.3</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="F60" t="n">
-        <v>0.4</v>
+        <v>-1.7</v>
       </c>
       <c r="G60" t="n">
-        <v>-0.445</v>
+        <v>-0.121</v>
       </c>
       <c r="H60" t="n">
-        <v>-0.454</v>
+        <v>0.485</v>
       </c>
       <c r="I60" t="n">
-        <v>73.3</v>
+        <v>-14.6</v>
       </c>
       <c r="J60" t="n">
-        <v>86.5</v>
+        <v>-11.8</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>688516.SH</t>
+          <t>688777.SH</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>奥特维</t>
+          <t>中控技术</t>
         </is>
       </c>
       <c r="C61" s="2" t="n">
-        <v>46030</v>
+        <v>46032</v>
       </c>
       <c r="D61" t="n">
-        <v>3.9</v>
+        <v>3.3</v>
       </c>
       <c r="E61" t="n">
-        <v>164.9</v>
+        <v>424.4</v>
       </c>
       <c r="F61" t="n">
-        <v>0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="G61" t="n">
-        <v>-0.415</v>
+        <v>-1.028</v>
       </c>
       <c r="H61" t="n">
-        <v>-0.08699999999999999</v>
+        <v>-1.215</v>
       </c>
       <c r="I61" t="n">
-        <v>41.9</v>
+        <v>129.5</v>
       </c>
       <c r="J61" t="n">
-        <v>80.3</v>
+        <v>2416.8</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>002258.SZ</t>
+          <t>002925.SZ</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>利尔化学</t>
+          <t>盈趣科技</t>
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>46029</v>
+        <v>46031</v>
       </c>
       <c r="D62" t="n">
-        <v>4.6</v>
+        <v>2.2</v>
       </c>
       <c r="E62" t="n">
-        <v>108.6</v>
+        <v>156.1</v>
       </c>
       <c r="F62" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="G62" t="n">
-        <v>-0.111</v>
+        <v>-0.445</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.347</v>
+        <v>0.363</v>
       </c>
       <c r="I62" t="n">
-        <v>23.6</v>
+        <v>71</v>
       </c>
       <c r="J62" t="n">
-        <v>32.3</v>
+        <v>80.2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>002080.SZ</t>
+          <t>300482.SZ</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>中材科技</t>
+          <t>万孚生物</t>
         </is>
       </c>
       <c r="C63" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D63" t="n">
-        <v>10.5</v>
+        <v>-0.2</v>
       </c>
       <c r="E63" t="n">
-        <v>637.4</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="F63" t="n">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="G63" t="n">
-        <v>-3.466</v>
+        <v>-1.888</v>
       </c>
       <c r="H63" t="n">
-        <v>-1.378</v>
+        <v>0.377</v>
       </c>
       <c r="I63" t="n">
-        <v>60.7</v>
+        <v>-629.4</v>
       </c>
       <c r="J63" t="n">
-        <v>-1209.7</v>
+        <v>-25.9</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>002204.SZ</t>
+          <t>300627.SZ</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>大连重工</t>
+          <t>华测导航</t>
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D64" t="n">
-        <v>3.6</v>
+        <v>6</v>
       </c>
       <c r="E64" t="n">
-        <v>146.4</v>
+        <v>326.9</v>
       </c>
       <c r="F64" t="n">
-        <v>-0.1</v>
+        <v>1.5</v>
       </c>
       <c r="G64" t="n">
-        <v>-1.178</v>
+        <v>-0.103</v>
       </c>
       <c r="H64" t="n">
-        <v>-1.095</v>
+        <v>-0.053</v>
       </c>
       <c r="I64" t="n">
-        <v>40.2</v>
+        <v>54.7</v>
       </c>
       <c r="J64" t="n">
-        <v>186.7</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>002444.SZ</t>
+          <t>300871.SZ</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>巨星科技</t>
+          <t>回盛生物</t>
         </is>
       </c>
       <c r="C65" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D65" t="n">
-        <v>23.1</v>
+        <v>2.1</v>
       </c>
       <c r="E65" t="n">
-        <v>408.9</v>
+        <v>45.4</v>
       </c>
       <c r="F65" t="n">
-        <v>2.7</v>
+        <v>0.5</v>
       </c>
       <c r="G65" t="n">
-        <v>-0.264</v>
+        <v>1.887</v>
       </c>
       <c r="H65" t="n">
-        <v>-0.65</v>
+        <v>-0.299</v>
       </c>
       <c r="I65" t="n">
-        <v>17.7</v>
+        <v>21.4</v>
       </c>
       <c r="J65" t="n">
-        <v>25.5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>002598.SZ</t>
+          <t>300887.SZ</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>山东章鼓</t>
+          <t>谱尼测试</t>
         </is>
       </c>
       <c r="C66" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D66" t="n">
-        <v>0.7</v>
+        <v>-2.6</v>
       </c>
       <c r="E66" t="n">
-        <v>30</v>
+        <v>87.2</v>
       </c>
       <c r="F66" t="n">
-        <v>0.1</v>
+        <v>-0.6</v>
       </c>
       <c r="G66" t="n">
-        <v>-1.408</v>
+        <v>-0.5590000000000001</v>
       </c>
       <c r="H66" t="n">
-        <v>-0.447</v>
+        <v>1.762</v>
       </c>
       <c r="I66" t="n">
-        <v>45.5</v>
+        <v>-33.4</v>
       </c>
       <c r="J66" t="n">
-        <v>55.4</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>002757.SZ</t>
+          <t>600340.SH</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>南兴股份</t>
+          <t>华夏幸福</t>
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D67" t="n">
-        <v>0.8</v>
+        <v>-250</v>
       </c>
       <c r="E67" t="n">
-        <v>63.3</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.1</v>
+        <v>-148.2</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.978</v>
+        <v>2.799</v>
       </c>
       <c r="H67" t="n">
-        <v>-1.313</v>
+        <v>4.994</v>
       </c>
       <c r="I67" t="n">
-        <v>84.40000000000001</v>
+        <v>-0.4</v>
       </c>
       <c r="J67" t="n">
-        <v>3773.1</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>002846.SZ</t>
+          <t>601872.SH</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>英联股份</t>
+          <t>招商轮船</t>
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2</v>
+        <v>50.1</v>
       </c>
       <c r="E68" t="n">
-        <v>70</v>
+        <v>775.2</v>
       </c>
       <c r="F68" t="n">
-        <v>-0.1</v>
+        <v>21</v>
       </c>
       <c r="G68" t="n">
-        <v>-0.845</v>
+        <v>0.218</v>
       </c>
       <c r="H68" t="n">
-        <v>-1.919</v>
+        <v>1.115</v>
       </c>
       <c r="I68" t="n">
-        <v>346.6</v>
+        <v>15.5</v>
       </c>
       <c r="J68" t="n">
-        <v>-550.7</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>300435.SZ</t>
+          <t>603895.SH</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>中泰股份</t>
+          <t>天永智能</t>
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D69" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>91.40000000000001</v>
+        <v>33.5</v>
       </c>
       <c r="F69" t="n">
-        <v>0.8</v>
+        <v>-0.1</v>
       </c>
       <c r="G69" t="n">
-        <v>-1.286</v>
+        <v>-0.961</v>
       </c>
       <c r="H69" t="n">
-        <v>-0.594</v>
+        <v>-3.763</v>
       </c>
       <c r="I69" t="n">
-        <v>22.7</v>
+        <v>836.3</v>
       </c>
       <c r="J69" t="n">
-        <v>20.9</v>
+        <v>-204.5</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>301345.SZ</t>
+          <t>688362.SH</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>涛涛车业</t>
+          <t>甬矽电子</t>
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>46028</v>
+        <v>46031</v>
       </c>
       <c r="D70" t="n">
-        <v>7.9</v>
+        <v>-0.5</v>
       </c>
       <c r="E70" t="n">
-        <v>280.9</v>
+        <v>167.4</v>
       </c>
       <c r="F70" t="n">
-        <v>1.9</v>
+        <v>-0.2</v>
       </c>
       <c r="G70" t="n">
-        <v>0.487</v>
+        <v>-20.432</v>
       </c>
       <c r="H70" t="n">
-        <v>-0.289</v>
+        <v>-2.607</v>
       </c>
       <c r="I70" t="n">
-        <v>35.6</v>
+        <v>-334.7</v>
       </c>
       <c r="J70" t="n">
-        <v>34.1</v>
+        <v>-388.9</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>600983.SH</t>
+          <t>300389.SZ</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>惠而浦</t>
+          <t>艾比森</t>
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>46028</v>
+        <v>46030</v>
       </c>
       <c r="D71" t="n">
-        <v>4.6</v>
+        <v>2.2</v>
       </c>
       <c r="E71" t="n">
-        <v>75</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="F71" t="n">
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="G71" t="n">
-        <v>0.08799999999999999</v>
+        <v>-21.933</v>
       </c>
       <c r="H71" t="n">
-        <v>0.658</v>
+        <v>0.005</v>
       </c>
       <c r="I71" t="n">
-        <v>16.5</v>
+        <v>29.6</v>
       </c>
       <c r="J71" t="n">
-        <v>13.3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>600988.SH</t>
+          <t>300498.SZ</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>赤峰黄金</t>
+          <t>温氏股份</t>
         </is>
       </c>
       <c r="C72" s="2" t="n">
-        <v>46028</v>
+        <v>46030</v>
       </c>
       <c r="D72" t="n">
-        <v>29.7</v>
+        <v>48</v>
       </c>
       <c r="E72" t="n">
-        <v>607.9</v>
+        <v>1125.2</v>
       </c>
       <c r="F72" t="n">
-        <v>9.4</v>
+        <v>-0.9</v>
       </c>
       <c r="G72" t="n">
-        <v>0.426</v>
+        <v>-1.029</v>
       </c>
       <c r="H72" t="n">
-        <v>0.033</v>
+        <v>-1.054</v>
       </c>
       <c r="I72" t="n">
-        <v>20.5</v>
+        <v>23.4</v>
       </c>
       <c r="J72" t="n">
-        <v>16.2</v>
+        <v>82.3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>603799.SH</t>
+          <t>300505.SZ</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>华友钴业</t>
+          <t>川金诺</t>
         </is>
       </c>
       <c r="C73" s="2" t="n">
-        <v>46028</v>
+        <v>46030</v>
       </c>
       <c r="D73" t="n">
-        <v>56</v>
+        <v>4.2</v>
       </c>
       <c r="E73" t="n">
-        <v>1289.8</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="F73" t="n">
-        <v>15.9</v>
+        <v>1.2</v>
       </c>
       <c r="G73" t="n">
-        <v>1.107</v>
+        <v>0.883</v>
       </c>
       <c r="H73" t="n">
-        <v>0.114</v>
+        <v>0.001</v>
       </c>
       <c r="I73" t="n">
-        <v>23</v>
+        <v>15.7</v>
       </c>
       <c r="J73" t="n">
-        <v>20.8</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>003017.SZ</t>
+          <t>300748.SZ</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>大洋生物</t>
+          <t>金力永磁</t>
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="D74" t="n">
-        <v>0.9</v>
+        <v>5.8</v>
       </c>
       <c r="E74" t="n">
-        <v>25.1</v>
+        <v>502.2</v>
       </c>
       <c r="F74" t="n">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
       <c r="G74" t="n">
-        <v>0.157</v>
+        <v>0.85</v>
       </c>
       <c r="H74" t="n">
-        <v>-0.468</v>
+        <v>-0.236</v>
       </c>
       <c r="I74" t="n">
-        <v>27.9</v>
+        <v>86.59999999999999</v>
       </c>
       <c r="J74" t="n">
-        <v>34.2</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>300428.SZ</t>
+          <t>300905.SZ</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>立中集团</t>
+          <t>宝丽迪</t>
         </is>
       </c>
       <c r="C75" s="2" t="n">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="D75" t="n">
-        <v>7.5</v>
+        <v>1.4</v>
       </c>
       <c r="E75" t="n">
-        <v>160.1</v>
+        <v>60.9</v>
       </c>
       <c r="F75" t="n">
-        <v>1.9</v>
+        <v>0.4</v>
       </c>
       <c r="G75" t="n">
-        <v>0.103</v>
+        <v>0.186</v>
       </c>
       <c r="H75" t="n">
-        <v>-0.048</v>
+        <v>-0.089</v>
       </c>
       <c r="I75" t="n">
-        <v>21.3</v>
+        <v>43.2</v>
       </c>
       <c r="J75" t="n">
-        <v>20.8</v>
+        <v>38.9</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>301377.SZ</t>
+          <t>600189.SH</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>鼎泰高科</t>
+          <t>泉阳泉</t>
         </is>
       </c>
       <c r="C76" s="2" t="n">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="D76" t="n">
-        <v>3.8</v>
+        <v>-0.2</v>
       </c>
       <c r="E76" t="n">
-        <v>570.3</v>
+        <v>49.9</v>
       </c>
       <c r="F76" t="n">
-        <v>1.2</v>
+        <v>-0.1</v>
       </c>
       <c r="G76" t="n">
-        <v>1.096</v>
+        <v>-0.778</v>
       </c>
       <c r="H76" t="n">
-        <v>0.022</v>
+        <v>0.046</v>
       </c>
       <c r="I76" t="n">
-        <v>150.1</v>
+        <v>-316.8</v>
       </c>
       <c r="J76" t="n">
-        <v>122.1</v>
+        <v>-96</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>301606.SZ</t>
+          <t>600435.SH</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>绿联科技</t>
+          <t>北方导航</t>
         </is>
       </c>
       <c r="C77" s="2" t="n">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="D77" t="n">
-        <v>6.2</v>
+        <v>0.9</v>
       </c>
       <c r="E77" t="n">
-        <v>243.7</v>
+        <v>299.7</v>
       </c>
       <c r="F77" t="n">
-        <v>1.8</v>
+        <v>-0.3</v>
       </c>
       <c r="G77" t="n">
-        <v>0.346</v>
+        <v>-1.216</v>
       </c>
       <c r="H77" t="n">
-        <v>-0.06</v>
+        <v>-6.115</v>
       </c>
       <c r="I77" t="n">
-        <v>39.1</v>
+        <v>336.8</v>
       </c>
       <c r="J77" t="n">
-        <v>34</v>
+        <v>-382.5</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>601339.SH</t>
+          <t>600500.SH</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>百隆东方</t>
+          <t>中化国际</t>
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>46027</v>
+        <v>46030</v>
       </c>
       <c r="D78" t="n">
-        <v>5.5</v>
+        <v>-23</v>
       </c>
       <c r="E78" t="n">
-        <v>86.8</v>
+        <v>145.3</v>
       </c>
       <c r="F78" t="n">
-        <v>0.4</v>
+        <v>-10</v>
       </c>
       <c r="G78" t="n">
-        <v>-2.161</v>
+        <v>-0.572</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.722</v>
+        <v>1.206</v>
       </c>
       <c r="I78" t="n">
-        <v>15.8</v>
+        <v>-6.3</v>
       </c>
       <c r="J78" t="n">
-        <v>31.9</v>
+        <v>-4.2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>000792.SZ</t>
+          <t>600537.SH</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>盐湖股份</t>
+          <t>亿晶光电</t>
         </is>
       </c>
       <c r="C79" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D79" t="n">
-        <v>82.3</v>
+        <v>-6</v>
       </c>
       <c r="E79" t="n">
-        <v>1467.9</v>
+        <v>51</v>
       </c>
       <c r="F79" t="n">
-        <v>37.4</v>
+        <v>-3.9</v>
       </c>
       <c r="G79" t="n">
-        <v>1.809</v>
+        <v>-0.746</v>
       </c>
       <c r="H79" t="n">
-        <v>0.882</v>
+        <v>5.3</v>
       </c>
       <c r="I79" t="n">
-        <v>17.8</v>
+        <v>-8.5</v>
       </c>
       <c r="J79" t="n">
-        <v>11.1</v>
+        <v>-4.2</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>000932.SZ</t>
+          <t>603309.SH</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>华菱钢铁</t>
+          <t>维力医疗</t>
         </is>
       </c>
       <c r="C80" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D80" t="n">
-        <v>23</v>
+        <v>0.6</v>
       </c>
       <c r="E80" t="n">
-        <v>386.9</v>
+        <v>41.4</v>
       </c>
       <c r="F80" t="n">
-        <v>0.1</v>
+        <v>-1.2</v>
       </c>
       <c r="G80" t="n">
-        <v>-1.036</v>
+        <v>-3.387</v>
       </c>
       <c r="H80" t="n">
-        <v>-0.991</v>
+        <v>-2.788</v>
       </c>
       <c r="I80" t="n">
-        <v>16.8</v>
+        <v>63.7</v>
       </c>
       <c r="J80" t="n">
-        <v>48.9</v>
+        <v>-14.2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>000959.SZ</t>
+          <t>603588.SH</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>首钢股份</t>
+          <t>高能环境</t>
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D81" t="n">
-        <v>9.199999999999999</v>
+        <v>7.5</v>
       </c>
       <c r="E81" t="n">
-        <v>380</v>
+        <v>126.1</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.7</v>
+        <v>1.5</v>
       </c>
       <c r="G81" t="n">
-        <v>-1.327</v>
+        <v>-2.068</v>
       </c>
       <c r="H81" t="n">
-        <v>-1.232</v>
+        <v>0.037</v>
       </c>
       <c r="I81" t="n">
-        <v>41.4</v>
+        <v>16.8</v>
       </c>
       <c r="J81" t="n">
-        <v>410.1</v>
+        <v>21.1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>002010.SZ</t>
+          <t>603589.SH</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>传化智联</t>
+          <t>口子窖</t>
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D82" t="n">
-        <v>3.2</v>
+        <v>6.5</v>
       </c>
       <c r="E82" t="n">
-        <v>161.7</v>
+        <v>181.3</v>
       </c>
       <c r="F82" t="n">
-        <v>-0.6</v>
+        <v>-0.8</v>
       </c>
       <c r="G82" t="n">
-        <v>-0.596</v>
+        <v>-1.231</v>
       </c>
       <c r="H82" t="n">
-        <v>-1.603</v>
+        <v>-3.991</v>
       </c>
       <c r="I82" t="n">
-        <v>50.5</v>
+        <v>28.1</v>
       </c>
       <c r="J82" t="n">
-        <v>-204.9</v>
+        <v>-85.5</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>002709.SZ</t>
+          <t>603590.SH</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>天赐材料</t>
+          <t>康辰药业</t>
         </is>
       </c>
       <c r="C83" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D83" t="n">
-        <v>10.5</v>
+        <v>1.4</v>
       </c>
       <c r="E83" t="n">
-        <v>922.6</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="F83" t="n">
-        <v>6.8</v>
+        <v>0.1</v>
       </c>
       <c r="G83" t="n">
-        <v>6.137</v>
+        <v>-1.093</v>
       </c>
       <c r="H83" t="n">
-        <v>3.884</v>
+        <v>-0.8100000000000001</v>
       </c>
       <c r="I83" t="n">
-        <v>87.90000000000001</v>
+        <v>47.6</v>
       </c>
       <c r="J83" t="n">
-        <v>42.5</v>
+        <v>115.4</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>300620.SZ</t>
+          <t>688332.SH</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>光库科技</t>
+          <t>中科蓝讯</t>
         </is>
       </c>
       <c r="C84" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D84" t="n">
-        <v>1.3</v>
+        <v>2.2</v>
       </c>
       <c r="E84" t="n">
-        <v>385</v>
+        <v>161.3</v>
       </c>
       <c r="F84" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G84" t="n">
-        <v>12.814</v>
+        <v>-0.445</v>
       </c>
       <c r="H84" t="n">
-        <v>0.143</v>
+        <v>-0.454</v>
       </c>
       <c r="I84" t="n">
-        <v>287.1</v>
+        <v>73.3</v>
       </c>
       <c r="J84" t="n">
-        <v>201.3</v>
+        <v>86.5</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>301078.SZ</t>
+          <t>688516.SH</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>孩子王</t>
+          <t>奥特维</t>
         </is>
       </c>
       <c r="C85" s="2" t="n">
-        <v>46022</v>
+        <v>46030</v>
       </c>
       <c r="D85" t="n">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="E85" t="n">
-        <v>129.8</v>
+        <v>164.9</v>
       </c>
       <c r="F85" t="n">
         <v>0.5</v>
       </c>
       <c r="G85" t="n">
-        <v>0.806</v>
+        <v>-0.415</v>
       </c>
       <c r="H85" t="n">
-        <v>0.194</v>
+        <v>-0.08699999999999999</v>
       </c>
       <c r="I85" t="n">
-        <v>63.3</v>
+        <v>41.9</v>
       </c>
       <c r="J85" t="n">
-        <v>68.90000000000001</v>
+        <v>80.3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>601899.SH</t>
+          <t>002258.SZ</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>紫金矿业</t>
+          <t>利尔化学</t>
         </is>
       </c>
       <c r="C86" s="2" t="n">
-        <v>46022</v>
+        <v>46029</v>
       </c>
       <c r="D86" t="n">
-        <v>475</v>
+        <v>4.6</v>
       </c>
       <c r="E86" t="n">
-        <v>8886.299999999999</v>
+        <v>108.6</v>
       </c>
       <c r="F86" t="n">
-        <v>133.7</v>
+        <v>0.7</v>
       </c>
       <c r="G86" t="n">
-        <v>0.6830000000000001</v>
+        <v>-0.111</v>
       </c>
       <c r="H86" t="n">
-        <v>0.07000000000000001</v>
+        <v>-0.347</v>
       </c>
       <c r="I86" t="n">
-        <v>18.7</v>
+        <v>23.6</v>
       </c>
       <c r="J86" t="n">
-        <v>16.9</v>
+        <v>32.3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>002080.SZ</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>中材科技</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D87" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E87" t="n">
+        <v>637.4</v>
+      </c>
+      <c r="F87" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="G87" t="n">
+        <v>-3.466</v>
+      </c>
+      <c r="H87" t="n">
+        <v>-1.378</v>
+      </c>
+      <c r="I87" t="n">
+        <v>60.7</v>
+      </c>
+      <c r="J87" t="n">
+        <v>-1209.7</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>002204.SZ</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>大连重工</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D88" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="E88" t="n">
+        <v>146.4</v>
+      </c>
+      <c r="F88" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="G88" t="n">
+        <v>-1.178</v>
+      </c>
+      <c r="H88" t="n">
+        <v>-1.095</v>
+      </c>
+      <c r="I88" t="n">
+        <v>40.2</v>
+      </c>
+      <c r="J88" t="n">
+        <v>186.7</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>002444.SZ</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>巨星科技</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D89" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="E89" t="n">
+        <v>408.9</v>
+      </c>
+      <c r="F89" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="G89" t="n">
+        <v>-0.264</v>
+      </c>
+      <c r="H89" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="I89" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="J89" t="n">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>002598.SZ</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>山东章鼓</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E90" t="n">
+        <v>30</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G90" t="n">
+        <v>-1.408</v>
+      </c>
+      <c r="H90" t="n">
+        <v>-0.447</v>
+      </c>
+      <c r="I90" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="J90" t="n">
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>002757.SZ</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>南兴股份</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E91" t="n">
+        <v>63.3</v>
+      </c>
+      <c r="F91" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="G91" t="n">
+        <v>-0.978</v>
+      </c>
+      <c r="H91" t="n">
+        <v>-1.313</v>
+      </c>
+      <c r="I91" t="n">
+        <v>84.40000000000001</v>
+      </c>
+      <c r="J91" t="n">
+        <v>3773.1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>002846.SZ</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>英联股份</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E92" t="n">
+        <v>70</v>
+      </c>
+      <c r="F92" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="G92" t="n">
+        <v>-0.845</v>
+      </c>
+      <c r="H92" t="n">
+        <v>-1.919</v>
+      </c>
+      <c r="I92" t="n">
+        <v>346.6</v>
+      </c>
+      <c r="J92" t="n">
+        <v>-550.7</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>300435.SZ</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>中泰股份</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D93" t="n">
+        <v>4</v>
+      </c>
+      <c r="E93" t="n">
+        <v>91.40000000000001</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G93" t="n">
+        <v>-1.286</v>
+      </c>
+      <c r="H93" t="n">
+        <v>-0.594</v>
+      </c>
+      <c r="I93" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="J93" t="n">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>301345.SZ</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>涛涛车业</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D94" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E94" t="n">
+        <v>280.9</v>
+      </c>
+      <c r="F94" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.487</v>
+      </c>
+      <c r="H94" t="n">
+        <v>-0.289</v>
+      </c>
+      <c r="I94" t="n">
+        <v>35.6</v>
+      </c>
+      <c r="J94" t="n">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>600983.SH</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>惠而浦</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D95" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="E95" t="n">
+        <v>75</v>
+      </c>
+      <c r="F95" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="I95" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="J95" t="n">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>600988.SH</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>赤峰黄金</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D96" t="n">
+        <v>29.7</v>
+      </c>
+      <c r="E96" t="n">
+        <v>607.9</v>
+      </c>
+      <c r="F96" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.426</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="I96" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="J96" t="n">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>603799.SH</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>华友钴业</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="D97" t="n">
+        <v>56</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1289.8</v>
+      </c>
+      <c r="F97" t="n">
+        <v>15.9</v>
+      </c>
+      <c r="G97" t="n">
+        <v>1.107</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="I97" t="n">
+        <v>23</v>
+      </c>
+      <c r="J97" t="n">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>003017.SZ</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>大洋生物</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E98" t="n">
+        <v>25.1</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.157</v>
+      </c>
+      <c r="H98" t="n">
+        <v>-0.468</v>
+      </c>
+      <c r="I98" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="J98" t="n">
+        <v>34.2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>300428.SZ</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>立中集团</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="D99" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E99" t="n">
+        <v>160.1</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="H99" t="n">
+        <v>-0.048</v>
+      </c>
+      <c r="I99" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="J99" t="n">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>301377.SZ</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>鼎泰高科</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="D100" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E100" t="n">
+        <v>570.3</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1.096</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="I100" t="n">
+        <v>150.1</v>
+      </c>
+      <c r="J100" t="n">
+        <v>122.1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>301606.SZ</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>绿联科技</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="D101" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E101" t="n">
+        <v>243.7</v>
+      </c>
+      <c r="F101" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.346</v>
+      </c>
+      <c r="H101" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="I101" t="n">
+        <v>39.1</v>
+      </c>
+      <c r="J101" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>601339.SH</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>百隆东方</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="D102" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E102" t="n">
+        <v>86.8</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G102" t="n">
+        <v>-2.161</v>
+      </c>
+      <c r="H102" t="n">
+        <v>-0.722</v>
+      </c>
+      <c r="I102" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="J102" t="n">
+        <v>31.9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>000792.SZ</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>盐湖股份</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D103" t="n">
+        <v>82.3</v>
+      </c>
+      <c r="E103" t="n">
+        <v>1467.9</v>
+      </c>
+      <c r="F103" t="n">
+        <v>37.4</v>
+      </c>
+      <c r="G103" t="n">
+        <v>1.809</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.882</v>
+      </c>
+      <c r="I103" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="J103" t="n">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>000932.SZ</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>华菱钢铁</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D104" t="n">
+        <v>23</v>
+      </c>
+      <c r="E104" t="n">
+        <v>386.9</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G104" t="n">
+        <v>-1.036</v>
+      </c>
+      <c r="H104" t="n">
+        <v>-0.991</v>
+      </c>
+      <c r="I104" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="J104" t="n">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>000959.SZ</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>首钢股份</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D105" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="E105" t="n">
+        <v>380</v>
+      </c>
+      <c r="F105" t="n">
+        <v>-0.7</v>
+      </c>
+      <c r="G105" t="n">
+        <v>-1.327</v>
+      </c>
+      <c r="H105" t="n">
+        <v>-1.232</v>
+      </c>
+      <c r="I105" t="n">
+        <v>41.4</v>
+      </c>
+      <c r="J105" t="n">
+        <v>410.1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>002010.SZ</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>传化智联</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D106" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="E106" t="n">
+        <v>161.7</v>
+      </c>
+      <c r="F106" t="n">
+        <v>-0.6</v>
+      </c>
+      <c r="G106" t="n">
+        <v>-0.596</v>
+      </c>
+      <c r="H106" t="n">
+        <v>-1.603</v>
+      </c>
+      <c r="I106" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="J106" t="n">
+        <v>-204.9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>002709.SZ</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>天赐材料</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D107" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E107" t="n">
+        <v>922.6</v>
+      </c>
+      <c r="F107" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="G107" t="n">
+        <v>6.137</v>
+      </c>
+      <c r="H107" t="n">
+        <v>3.884</v>
+      </c>
+      <c r="I107" t="n">
+        <v>87.90000000000001</v>
+      </c>
+      <c r="J107" t="n">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>300620.SZ</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>光库科技</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E108" t="n">
+        <v>385</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G108" t="n">
+        <v>12.814</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="I108" t="n">
+        <v>287.1</v>
+      </c>
+      <c r="J108" t="n">
+        <v>201.3</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>301078.SZ</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>孩子王</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D109" t="n">
+        <v>2</v>
+      </c>
+      <c r="E109" t="n">
+        <v>129.8</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.806</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="I109" t="n">
+        <v>63.3</v>
+      </c>
+      <c r="J109" t="n">
+        <v>68.90000000000001</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>601899.SH</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>紫金矿业</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>46022</v>
+      </c>
+      <c r="D110" t="n">
+        <v>475</v>
+      </c>
+      <c r="E110" t="n">
+        <v>8886.299999999999</v>
+      </c>
+      <c r="F110" t="n">
+        <v>133.7</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.6830000000000001</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I110" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="J110" t="n">
+        <v>16.9</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
           <t>002050.SZ</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B111" t="inlineStr">
         <is>
           <t>三花智控</t>
         </is>
       </c>
-      <c r="C87" s="2" t="n">
+      <c r="C111" s="2" t="n">
         <v>46014</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D111" t="n">
         <v>36.8</v>
       </c>
-      <c r="E87" t="n">
+      <c r="E111" t="n">
         <v>1911.3</v>
       </c>
-      <c r="F87" t="n">
+      <c r="F111" t="n">
         <v>6</v>
       </c>
-      <c r="G87" t="n">
+      <c r="G111" t="n">
         <v>-0.315</v>
       </c>
-      <c r="H87" t="n">
+      <c r="H111" t="n">
         <v>-0.445</v>
       </c>
-      <c r="I87" t="n">
+      <c r="I111" t="n">
         <v>51.9</v>
       </c>
-      <c r="J87" t="n">
+      <c r="J111" t="n">
         <v>66.8</v>
       </c>
     </row>

</xml_diff>